<commit_message>
Delete 6.8.2(3.75)_8sfpp; Edit ATT inits; Edit CBL15 (OD AC)
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL15.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541D09BA-8A90-4721-92D3-DF45BCF373F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CBEB10-772D-4893-A20B-08472FE5E83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="1515" windowWidth="21945" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="690" windowWidth="21945" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,13 +61,7 @@
     <t>Qty for Tester</t>
   </si>
   <si>
-    <t>red</t>
-  </si>
-  <si>
     <t>yellow-green</t>
-  </si>
-  <si>
-    <t>black</t>
   </si>
   <si>
     <t>Cable Name: AT-ETX-2i10G/CBL15</t>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t>Please attach a label the with Cable Name to the cable</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>blue</t>
   </si>
 </sst>
 </file>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="21"/>
     </row>
@@ -711,7 +711,7 @@
     <row r="3" spans="1:4" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="18"/>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" s="5"/>
     </row>
@@ -854,7 +854,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2">
         <v>3</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -890,19 +890,19 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>720</v>
+        <v>640</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Init; change cable-15
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL15.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CBEB10-772D-4893-A20B-08472FE5E83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013C71B7-A007-45DF-B0EA-C4815484F1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="690" windowWidth="21945" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7395" yWindow="1155" windowWidth="19230" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D23" s="5"/>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="D27" s="2">
         <f>$C$23*C27</f>
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
       </c>
       <c r="D28" s="2">
         <f>$C$23*C28</f>
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
       </c>
       <c r="D29" s="2">
         <f t="shared" ref="D29:D30" si="0">$C$23*C29</f>
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change quantity to 8
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL15.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013C71B7-A007-45DF-B0EA-C4815484F1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418DF8A7-A10A-45BE-BB29-8FE4F8B4F182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="1155" windowWidth="19230" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33240" yWindow="765" windowWidth="19230" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -823,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="3">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D23" s="5"/>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="D27" s="2">
         <f>$C$23*C27</f>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
       </c>
       <c r="D28" s="2">
         <f>$C$23*C28</f>
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
       </c>
       <c r="D29" s="2">
         <f t="shared" ref="D29:D30" si="0">$C$23*C29</f>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>640</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>